<commit_message>
Class -> SchoolClass, Migrations neu angelegt, TestFillDb funktioniert, Web Projekt gelöscht
</commit_message>
<xml_diff>
--- a/01_Planning/SprintLog.xlsx
+++ b/01_Planning/SprintLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Sprint Log</t>
   </si>
@@ -51,6 +51,30 @@
   </si>
   <si>
     <t>Effort</t>
+  </si>
+  <si>
+    <t>Log</t>
+  </si>
+  <si>
+    <t>Woche</t>
+  </si>
+  <si>
+    <t>Getan</t>
+  </si>
+  <si>
+    <t>bis 25.4</t>
+  </si>
+  <si>
+    <t>Eva</t>
+  </si>
+  <si>
+    <t>Danijal</t>
+  </si>
+  <si>
+    <t>Layoutänderungen in Index</t>
+  </si>
+  <si>
+    <t>Testdatensätze eingefügt, FillDb funktioniert;Probleme beim Login: Zertifikat nicht gültig</t>
   </si>
 </sst>
 </file>
@@ -369,23 +393,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:H5"/>
+  <dimension ref="C2:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="60.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>0</v>
       </c>
+      <c r="L2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>1</v>
       </c>
@@ -404,8 +432,17 @@
       <c r="H4" t="s">
         <v>8</v>
       </c>
+      <c r="L4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>1</v>
       </c>
@@ -423,6 +460,23 @@
       </c>
       <c r="H5">
         <v>3</v>
+      </c>
+      <c r="L5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>